<commit_message>
modify Config files, try automatic code generation.
</commit_message>
<xml_diff>
--- a/Source/Extend/Driver/Config/gpio_Config.xlsx
+++ b/Source/Extend/Driver/Config/gpio_Config.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE7AC2E9-D73E-4EED-B5D1-619E8185564B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GPIO" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,14 +19,66 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>GPIOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIOx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PINx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IN/OUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PULL/DROP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SET/RESET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -330,13 +383,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>